<commit_message>
BIS-1439: Changed the name of a test file not to collide with an existing one in a productive instance. This is to avoid a potential bug report if an inline file with exactly the same name will be exported.
</commit_message>
<xml_diff>
--- a/openbis/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/import_inlined_image_cell.xlsx
+++ b/openbis/sourceTest/java/ch/ethz/sis/openbis/systemtest/asapi/v3/test_files/import/import_inlined_image_cell.xlsx
@@ -303,7 +303,7 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;html&gt;&lt;head&gt;&lt;/head&gt;&lt;body&gt;&lt;figure class="image image-style-align-left image_resized" style="width:94.98%;"&gt;&lt;img src="/openbis/openbis/file-service/eln-lims/13/3d/d4/133dd458-9f7f-4ca9-8353-9de3f00f2a55/78397d5b-fe0d-45e8-9f1c-9fa665bc81e3.png" /&gt;&lt;figcaption&gt;Print Picture Screen NanoDrop&lt;/figcaption&gt;&lt;/figure&gt;&lt;p&gt; &lt;/p&gt;&lt;p&gt; &lt;/p&gt;&lt;p&gt; &lt;/p&gt;&lt;/body&gt;&lt;/html&gt;</t>
+&lt;html&gt;&lt;head&gt;&lt;/head&gt;&lt;body&gt;&lt;figure class="image image-style-align-left image_resized" style="width:94.98%;"&gt;&lt;img src="/openbis/openbis/file-service/eln-lims/98/05/3b/98053b86-36cb-4a74-a603-893a9a1c53bb/98053b86-36cb-4a74-a603-893a9a1c53bb.png" /&gt;&lt;figcaption&gt;Print Picture Screen NanoDrop&lt;/figcaption&gt;&lt;/figure&gt;&lt;p&gt; &lt;/p&gt;&lt;p&gt; &lt;/p&gt;&lt;p&gt; &lt;/p&gt;&lt;/body&gt;&lt;/html&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">VVV</t>
@@ -432,6 +432,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1294,13 +1295,13 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
+      <selection pane="topLeft" activeCell="M21" activeCellId="0" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="75.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="75.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="1" width="8.37"/>
   </cols>
   <sheetData>
@@ -1479,7 +1480,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>